<commit_message>
fix scrape id founders
</commit_message>
<xml_diff>
--- a/LinkedIn_RACollection_3045_RA.xlsx
+++ b/LinkedIn_RACollection_3045_RA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\KERJA\BOT\LinkedInScraper\LinkedinScraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D6CB5C-1B5F-42C4-85A0-4985C91F3A85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29808CFD-F169-4A35-BB11-EEB9FA77AFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E782CB89-4562-B448-9DF1-2246441D2FCD}"/>
   </bookViews>
@@ -14032,12 +14032,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -14053,11 +14059,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -14426,8 +14433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B977671-7F1B-2440-BA23-BF40D7E48C50}">
   <dimension ref="A1:E1165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14530,7 +14537,7 @@
       <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D6">
@@ -14615,7 +14622,7 @@
       <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D11">
@@ -14632,7 +14639,7 @@
       <c r="B12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D12">
@@ -14683,7 +14690,7 @@
       <c r="B15" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D15">
@@ -15458,20 +15465,20 @@
         <v>240</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="4">
         <v>3</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="4" t="s">
         <v>244</v>
       </c>
     </row>
@@ -16196,7 +16203,7 @@
       <c r="B104" t="s">
         <v>414</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="1" t="s">
         <v>415</v>
       </c>
       <c r="D104">
@@ -16342,20 +16349,20 @@
         <v>448</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="113" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
         <v>449</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="4">
         <v>5</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="4" t="s">
         <v>452</v>
       </c>
     </row>
@@ -16655,7 +16662,7 @@
       <c r="B131" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="1" t="s">
         <v>523</v>
       </c>
       <c r="D131">
@@ -32431,7 +32438,7 @@
       <c r="B1059" t="s">
         <v>4233</v>
       </c>
-      <c r="C1059" t="s">
+      <c r="C1059" s="1" t="s">
         <v>4234</v>
       </c>
       <c r="D1059">
@@ -34286,6 +34293,13 @@
     <hyperlink ref="C70" r:id="rId24" xr:uid="{70C19E02-702D-094F-BC74-E2637CA9E0A5}"/>
     <hyperlink ref="C19" r:id="rId25" xr:uid="{41E4FC44-7021-4119-B3A5-5502B1E5446B}"/>
     <hyperlink ref="C21" r:id="rId26" xr:uid="{1CCB3E95-0406-4EA0-975D-D551AD1EE985}"/>
+    <hyperlink ref="C104" r:id="rId27" xr:uid="{7682B436-E7C7-4964-B4FB-560D5DD920A1}"/>
+    <hyperlink ref="C1059" r:id="rId28" xr:uid="{4979C176-B9A3-4FDE-8683-849C8A14ECC7}"/>
+    <hyperlink ref="C11" r:id="rId29" xr:uid="{EB71831E-2362-4CEE-BF9F-BB42B2EEC6C9}"/>
+    <hyperlink ref="C12" r:id="rId30" xr:uid="{35912ECE-5D95-4F0C-8A5D-600A3431CFCF}"/>
+    <hyperlink ref="C15" r:id="rId31" xr:uid="{39CD3A64-D4A5-4D29-8CC6-D0F765F26361}"/>
+    <hyperlink ref="C6" r:id="rId32" xr:uid="{EFEE5F3D-2D64-41F6-B914-79DB73645E52}"/>
+    <hyperlink ref="C131" r:id="rId33" xr:uid="{1493865B-95AC-47C5-9D77-8FD12A5994B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>